<commit_message>
Ajout modele + OJ
</commit_message>
<xml_diff>
--- a/meeting/GestionHedbo_Semaine4.xlsx
+++ b/meeting/GestionHedbo_Semaine4.xlsx
@@ -342,7 +342,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,6 +361,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="21">
     <border>
@@ -632,7 +638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -668,41 +674,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -723,50 +694,85 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -777,6 +783,8 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1080,17 +1088,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="36"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -1099,12 +1107,12 @@
       <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1125,15 +1133,15 @@
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1143,45 +1151,45 @@
       <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18" t="s">
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="18"/>
+      <c r="G5" s="40"/>
       <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="7"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
       <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="7"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
       <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
       <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1195,15 +1203,15 @@
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1231,7 +1239,7 @@
       <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8" s="4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="43" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1240,101 +1248,101 @@
       <c r="C12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="31"/>
-      <c r="E12" s="20">
+      <c r="D12" s="54"/>
+      <c r="E12" s="43">
         <v>158</v>
       </c>
       <c r="F12" s="10">
         <v>4</v>
       </c>
-      <c r="G12" s="20">
+      <c r="G12" s="43">
         <f>E12-SUM(F12:F17)</f>
         <v>143</v>
       </c>
       <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="20"/>
-      <c r="B13" s="29" t="s">
+      <c r="A13" s="43"/>
+      <c r="B13" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="20"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="43"/>
       <c r="F13" s="10">
         <v>3</v>
       </c>
-      <c r="G13" s="20"/>
+      <c r="G13" s="43"/>
       <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="29" t="s">
+      <c r="A14" s="43"/>
+      <c r="B14" s="16" t="s">
         <v>41</v>
       </c>
       <c r="C14" s="11">
         <v>41336</v>
       </c>
-      <c r="D14" s="31"/>
-      <c r="E14" s="20"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="43"/>
       <c r="F14" s="10">
         <v>2</v>
       </c>
-      <c r="G14" s="20"/>
+      <c r="G14" s="43"/>
       <c r="H14" s="12"/>
     </row>
     <row r="15" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
-      <c r="B15" s="34" t="s">
+      <c r="A15" s="44"/>
+      <c r="B15" s="21" t="s">
         <v>53</v>
       </c>
       <c r="C15" s="11">
         <v>41336</v>
       </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="33">
+      <c r="D15" s="19"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="20">
         <v>1</v>
       </c>
-      <c r="G15" s="41"/>
+      <c r="G15" s="44"/>
       <c r="H15" s="12"/>
     </row>
     <row r="16" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="34" t="s">
+      <c r="A16" s="44"/>
+      <c r="B16" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="32"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="33">
+      <c r="D16" s="19"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="20">
         <v>3</v>
       </c>
-      <c r="G16" s="41"/>
+      <c r="G16" s="44"/>
       <c r="H16" s="12"/>
     </row>
     <row r="17" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="29" t="s">
+      <c r="A17" s="43"/>
+      <c r="B17" s="16" t="s">
         <v>44</v>
       </c>
       <c r="C17" s="11">
         <v>41336</v>
       </c>
-      <c r="D17" s="31"/>
-      <c r="E17" s="20"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="43"/>
       <c r="F17" s="10">
         <v>2</v>
       </c>
-      <c r="G17" s="20"/>
+      <c r="G17" s="43"/>
       <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8" s="4" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="43" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
@@ -1343,101 +1351,101 @@
       <c r="C18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="31"/>
-      <c r="E18" s="20">
+      <c r="D18" s="54"/>
+      <c r="E18" s="43">
         <v>169</v>
       </c>
       <c r="F18" s="10">
         <v>4</v>
       </c>
-      <c r="G18" s="20">
-        <f>(E18-F18)-F23</f>
-        <v>162</v>
+      <c r="G18" s="43">
+        <f>(E18-SUM(F18:F23))</f>
+        <v>155</v>
       </c>
       <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:8" s="4" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="34" t="s">
+      <c r="A19" s="44"/>
+      <c r="B19" s="21" t="s">
         <v>42</v>
       </c>
       <c r="C19" s="11">
         <v>41336</v>
       </c>
-      <c r="D19" s="32"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="33">
+      <c r="D19" s="19"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="20">
         <v>2</v>
       </c>
-      <c r="G19" s="41"/>
+      <c r="G19" s="44"/>
       <c r="H19" s="12"/>
     </row>
     <row r="20" spans="1:8" s="4" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
-      <c r="B20" s="34" t="s">
+      <c r="A20" s="44"/>
+      <c r="B20" s="21" t="s">
         <v>53</v>
       </c>
       <c r="C20" s="11">
         <v>41336</v>
       </c>
-      <c r="D20" s="32"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="33">
+      <c r="D20" s="19"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="20">
         <v>1</v>
       </c>
-      <c r="G20" s="41"/>
+      <c r="G20" s="44"/>
       <c r="H20" s="12"/>
     </row>
     <row r="21" spans="1:8" s="4" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="41"/>
-      <c r="B21" s="34" t="s">
+      <c r="A21" s="44"/>
+      <c r="B21" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="32"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="33">
+      <c r="D21" s="19"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="20">
         <v>3</v>
       </c>
-      <c r="G21" s="41"/>
+      <c r="G21" s="44"/>
       <c r="H21" s="12"/>
     </row>
     <row r="22" spans="1:8" s="4" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
-      <c r="B22" s="34" t="s">
+      <c r="A22" s="44"/>
+      <c r="B22" s="21" t="s">
         <v>50</v>
       </c>
       <c r="C22" s="11">
         <v>41336</v>
       </c>
-      <c r="D22" s="32"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="33">
+      <c r="D22" s="19"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="20">
         <v>1</v>
       </c>
-      <c r="G22" s="41"/>
+      <c r="G22" s="44"/>
       <c r="H22" s="12"/>
     </row>
     <row r="23" spans="1:8" s="4" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
-      <c r="B23" s="29" t="s">
+      <c r="A23" s="43"/>
+      <c r="B23" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="31"/>
-      <c r="E23" s="20"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="43"/>
       <c r="F23" s="10">
         <v>3</v>
       </c>
-      <c r="G23" s="20"/>
+      <c r="G23" s="43"/>
       <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="45" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="8" t="s">
@@ -1446,590 +1454,590 @@
       <c r="C24" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="31"/>
-      <c r="E24" s="20">
+      <c r="D24" s="54"/>
+      <c r="E24" s="43">
         <v>158</v>
       </c>
       <c r="F24" s="10">
         <v>4</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="45">
         <f>E24-SUM(F24:F28)</f>
         <v>145</v>
       </c>
       <c r="H24" s="12"/>
     </row>
     <row r="25" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
-      <c r="B25" s="34" t="s">
+      <c r="A25" s="46"/>
+      <c r="B25" s="21" t="s">
         <v>53</v>
       </c>
       <c r="C25" s="11">
         <v>41336</v>
       </c>
-      <c r="D25" s="32"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="33">
+      <c r="D25" s="19"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="20">
         <v>1</v>
       </c>
-      <c r="G25" s="42"/>
+      <c r="G25" s="46"/>
       <c r="H25" s="12"/>
     </row>
     <row r="26" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
-      <c r="B26" s="34" t="s">
+      <c r="A26" s="46"/>
+      <c r="B26" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="35" t="s">
+      <c r="C26" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="32"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="33">
+      <c r="D26" s="19"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="20">
         <v>2</v>
       </c>
-      <c r="G26" s="42"/>
+      <c r="G26" s="46"/>
       <c r="H26" s="12"/>
     </row>
     <row r="27" spans="1:8" s="4" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
-      <c r="B27" s="29" t="s">
+      <c r="A27" s="45"/>
+      <c r="B27" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="30" t="s">
+      <c r="C27" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D27" s="31"/>
-      <c r="E27" s="22"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="47"/>
       <c r="F27" s="10">
         <v>3</v>
       </c>
-      <c r="G27" s="19"/>
+      <c r="G27" s="45"/>
       <c r="H27" s="12"/>
     </row>
     <row r="28" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
-      <c r="B28" s="29" t="s">
+      <c r="A28" s="43"/>
+      <c r="B28" s="16" t="s">
         <v>45</v>
       </c>
       <c r="C28" s="11">
         <v>41336</v>
       </c>
-      <c r="D28" s="31"/>
-      <c r="E28" s="23"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="48"/>
       <c r="F28" s="10">
         <v>3</v>
       </c>
-      <c r="G28" s="20"/>
+      <c r="G28" s="43"/>
       <c r="H28" s="12"/>
     </row>
     <row r="29" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C29" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="32"/>
-      <c r="E29" s="38">
+      <c r="D29" s="55"/>
+      <c r="E29" s="24">
         <v>162</v>
       </c>
-      <c r="F29" s="33">
+      <c r="F29" s="20">
         <v>8</v>
       </c>
-      <c r="G29" s="38">
-        <f>E29-F33</f>
-        <v>159</v>
+      <c r="G29" s="24">
+        <f>E29-SUM(F29:F33)</f>
+        <v>145</v>
       </c>
       <c r="H29" s="12"/>
     </row>
     <row r="30" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="43"/>
-      <c r="B30" s="34" t="s">
+      <c r="A30" s="28"/>
+      <c r="B30" s="21" t="s">
         <v>53</v>
       </c>
       <c r="C30" s="11">
         <v>41336</v>
       </c>
-      <c r="D30" s="32"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="33">
+      <c r="D30" s="19"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="20">
         <v>1</v>
       </c>
-      <c r="G30" s="44"/>
+      <c r="G30" s="25"/>
       <c r="H30" s="12"/>
     </row>
     <row r="31" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="43"/>
-      <c r="B31" s="34" t="s">
+      <c r="A31" s="28"/>
+      <c r="B31" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C31" s="11">
         <v>41336</v>
       </c>
-      <c r="D31" s="32"/>
-      <c r="E31" s="44"/>
-      <c r="F31" s="33">
+      <c r="D31" s="19"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="20">
         <v>3</v>
       </c>
-      <c r="G31" s="44"/>
+      <c r="G31" s="25"/>
       <c r="H31" s="12"/>
     </row>
     <row r="32" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="43"/>
-      <c r="B32" s="34" t="s">
+      <c r="A32" s="28"/>
+      <c r="B32" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="35" t="s">
+      <c r="C32" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="32"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="33">
+      <c r="D32" s="19"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="20">
         <v>2</v>
       </c>
-      <c r="G32" s="44"/>
+      <c r="G32" s="25"/>
       <c r="H32" s="12"/>
     </row>
     <row r="33" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="37"/>
-      <c r="B33" s="29" t="s">
+      <c r="A33" s="29"/>
+      <c r="B33" s="16" t="s">
         <v>46</v>
       </c>
       <c r="C33" s="11">
         <v>41336</v>
       </c>
-      <c r="D33" s="31"/>
-      <c r="E33" s="39"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="26"/>
       <c r="F33" s="10">
         <v>3</v>
       </c>
-      <c r="G33" s="39"/>
+      <c r="G33" s="26"/>
       <c r="H33" s="12"/>
     </row>
     <row r="34" spans="1:8" s="4" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="31"/>
-      <c r="E34" s="19">
+      <c r="D34" s="54"/>
+      <c r="E34" s="45">
         <v>169</v>
       </c>
       <c r="F34" s="10">
         <v>4</v>
       </c>
-      <c r="G34" s="19">
-        <f>(E34-F34)-F38</f>
-        <v>162</v>
+      <c r="G34" s="45">
+        <f>(E34)-SUM(F34:F38)</f>
+        <v>156</v>
       </c>
       <c r="H34" s="12"/>
     </row>
     <row r="35" spans="1:8" s="4" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="39"/>
-      <c r="B35" s="34" t="s">
+      <c r="A35" s="26"/>
+      <c r="B35" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C35" s="11">
         <v>41336</v>
       </c>
-      <c r="D35" s="32"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="33">
+      <c r="D35" s="19"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="20">
         <v>3</v>
       </c>
-      <c r="G35" s="42"/>
+      <c r="G35" s="46"/>
       <c r="H35" s="12"/>
     </row>
     <row r="36" spans="1:8" s="4" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="39"/>
-      <c r="B36" s="34" t="s">
+      <c r="A36" s="26"/>
+      <c r="B36" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C36" s="35" t="s">
+      <c r="C36" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="D36" s="32"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="33">
+      <c r="D36" s="19"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="20">
         <v>2</v>
       </c>
-      <c r="G36" s="42"/>
+      <c r="G36" s="46"/>
       <c r="H36" s="12"/>
     </row>
     <row r="37" spans="1:8" s="4" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="39"/>
-      <c r="B37" s="34" t="s">
+      <c r="A37" s="26"/>
+      <c r="B37" s="21" t="s">
         <v>53</v>
       </c>
       <c r="C37" s="11">
         <v>41336</v>
       </c>
-      <c r="D37" s="32"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="33">
+      <c r="D37" s="19"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="20">
         <v>1</v>
       </c>
-      <c r="G37" s="42"/>
+      <c r="G37" s="46"/>
       <c r="H37" s="12"/>
     </row>
     <row r="38" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
-      <c r="B38" s="29" t="s">
+      <c r="A38" s="49"/>
+      <c r="B38" s="16" t="s">
         <v>48</v>
       </c>
       <c r="C38" s="11">
         <v>41336</v>
       </c>
-      <c r="D38" s="31"/>
-      <c r="E38" s="19"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="45"/>
       <c r="F38" s="10">
         <v>3</v>
       </c>
-      <c r="G38" s="19"/>
+      <c r="G38" s="45"/>
       <c r="H38" s="12"/>
     </row>
     <row r="39" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="B39" s="29" t="s">
+      <c r="B39" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="40" t="s">
+      <c r="C39" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D39" s="31"/>
-      <c r="E39" s="19">
+      <c r="D39" s="18"/>
+      <c r="E39" s="45">
         <v>163</v>
       </c>
       <c r="F39" s="10">
         <v>6</v>
       </c>
-      <c r="G39" s="19">
-        <f>(E39-F39)-F45</f>
-        <v>154</v>
+      <c r="G39" s="45">
+        <f>(E39)-SUM(F39:F45)</f>
+        <v>141</v>
       </c>
       <c r="H39" s="12"/>
     </row>
     <row r="40" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="42"/>
-      <c r="B40" s="34" t="s">
+      <c r="A40" s="46"/>
+      <c r="B40" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C40" s="11">
         <v>41336</v>
       </c>
-      <c r="D40" s="32"/>
-      <c r="E40" s="42"/>
-      <c r="F40" s="33">
+      <c r="D40" s="19"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="20">
         <v>3</v>
       </c>
-      <c r="G40" s="42"/>
+      <c r="G40" s="46"/>
       <c r="H40" s="12"/>
     </row>
     <row r="41" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="42"/>
-      <c r="B41" s="34" t="s">
+      <c r="A41" s="46"/>
+      <c r="B41" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C41" s="35" t="s">
+      <c r="C41" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="D41" s="32"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="33">
+      <c r="D41" s="19"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="20">
         <v>2</v>
       </c>
-      <c r="G41" s="42"/>
+      <c r="G41" s="46"/>
       <c r="H41" s="12"/>
     </row>
     <row r="42" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="42"/>
-      <c r="B42" s="34" t="s">
+      <c r="A42" s="46"/>
+      <c r="B42" s="21" t="s">
         <v>53</v>
       </c>
       <c r="C42" s="11">
         <v>41336</v>
       </c>
-      <c r="D42" s="32"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="33">
+      <c r="D42" s="19"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="20">
         <v>1</v>
       </c>
-      <c r="G42" s="42"/>
+      <c r="G42" s="46"/>
       <c r="H42" s="12"/>
     </row>
     <row r="43" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="42"/>
-      <c r="B43" s="29" t="s">
+      <c r="A43" s="46"/>
+      <c r="B43" s="16" t="s">
         <v>48</v>
       </c>
       <c r="C43" s="11">
         <v>41336</v>
       </c>
-      <c r="D43" s="32"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="33">
+      <c r="D43" s="19"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="20">
         <v>3</v>
       </c>
-      <c r="G43" s="42"/>
+      <c r="G43" s="46"/>
       <c r="H43" s="12"/>
     </row>
     <row r="44" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="42"/>
-      <c r="B44" s="34" t="s">
+      <c r="A44" s="46"/>
+      <c r="B44" s="21" t="s">
         <v>49</v>
       </c>
       <c r="C44" s="11">
         <v>41336</v>
       </c>
-      <c r="D44" s="32"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="33">
+      <c r="D44" s="19"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="20">
         <v>4</v>
       </c>
-      <c r="G44" s="42"/>
+      <c r="G44" s="46"/>
       <c r="H44" s="12"/>
     </row>
     <row r="45" spans="1:8" s="4" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="19"/>
-      <c r="B45" s="29" t="s">
+      <c r="A45" s="45"/>
+      <c r="B45" s="16" t="s">
         <v>25</v>
       </c>
       <c r="C45" s="11">
         <v>41336</v>
       </c>
-      <c r="D45" s="31"/>
-      <c r="E45" s="19"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="45"/>
       <c r="F45" s="10">
         <v>3</v>
       </c>
-      <c r="G45" s="19"/>
+      <c r="G45" s="45"/>
       <c r="H45" s="12"/>
     </row>
     <row r="46" spans="1:8" s="4" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="45" t="s">
+      <c r="A46" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B46" s="34" t="s">
+      <c r="B46" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C46" s="11">
         <v>41336</v>
       </c>
-      <c r="D46" s="32"/>
-      <c r="E46" s="48">
+      <c r="D46" s="19"/>
+      <c r="E46" s="33">
         <v>156</v>
       </c>
-      <c r="F46" s="33">
+      <c r="F46" s="20">
         <v>3</v>
       </c>
-      <c r="G46" s="48">
-        <f>(E46-F49)-F51</f>
-        <v>150</v>
+      <c r="G46" s="33">
+        <f>E46-SUM(F46:F51)</f>
+        <v>140</v>
       </c>
       <c r="H46" s="12"/>
     </row>
     <row r="47" spans="1:8" s="4" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="46"/>
-      <c r="B47" s="34" t="s">
+      <c r="A47" s="31"/>
+      <c r="B47" s="21" t="s">
         <v>53</v>
       </c>
       <c r="C47" s="11">
         <v>41336</v>
       </c>
-      <c r="D47" s="32"/>
-      <c r="E47" s="49"/>
-      <c r="F47" s="33">
+      <c r="D47" s="19"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="20">
         <v>1</v>
       </c>
-      <c r="G47" s="49"/>
+      <c r="G47" s="34"/>
       <c r="H47" s="12"/>
     </row>
     <row r="48" spans="1:8" s="4" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="46"/>
-      <c r="B48" s="34" t="s">
+      <c r="A48" s="31"/>
+      <c r="B48" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="40" t="s">
+      <c r="C48" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D48" s="32"/>
-      <c r="E48" s="49"/>
-      <c r="F48" s="33">
+      <c r="D48" s="19"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="20">
         <v>2</v>
       </c>
-      <c r="G48" s="49"/>
+      <c r="G48" s="34"/>
       <c r="H48" s="12"/>
     </row>
     <row r="49" spans="1:8" s="4" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="46"/>
-      <c r="B49" s="29" t="s">
+      <c r="A49" s="31"/>
+      <c r="B49" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C49" s="40" t="s">
+      <c r="C49" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D49" s="31"/>
-      <c r="E49" s="49"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="34"/>
       <c r="F49" s="10">
         <v>4</v>
       </c>
-      <c r="G49" s="49"/>
+      <c r="G49" s="34"/>
       <c r="H49" s="12"/>
     </row>
     <row r="50" spans="1:8" s="4" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="46"/>
-      <c r="B50" s="34" t="s">
+      <c r="A50" s="31"/>
+      <c r="B50" s="21" t="s">
         <v>51</v>
       </c>
       <c r="C50" s="11">
         <v>41336</v>
       </c>
-      <c r="D50" s="32"/>
-      <c r="E50" s="49"/>
-      <c r="F50" s="33">
+      <c r="D50" s="19"/>
+      <c r="E50" s="34"/>
+      <c r="F50" s="20">
         <v>4</v>
       </c>
-      <c r="G50" s="49"/>
+      <c r="G50" s="34"/>
       <c r="H50" s="12"/>
     </row>
     <row r="51" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="47"/>
-      <c r="B51" s="29" t="s">
+      <c r="A51" s="32"/>
+      <c r="B51" s="16" t="s">
         <v>47</v>
       </c>
       <c r="C51" s="11">
         <v>41336</v>
       </c>
-      <c r="D51" s="31"/>
-      <c r="E51" s="50"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="35"/>
       <c r="F51" s="10">
         <v>2</v>
       </c>
-      <c r="G51" s="50"/>
+      <c r="G51" s="35"/>
       <c r="H51" s="12"/>
     </row>
     <row r="52" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="38" t="s">
+      <c r="A52" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B52" s="34" t="s">
+      <c r="B52" s="21" t="s">
         <v>43</v>
       </c>
       <c r="C52" s="11">
         <v>41336</v>
       </c>
-      <c r="D52" s="32"/>
-      <c r="E52" s="48">
+      <c r="D52" s="19"/>
+      <c r="E52" s="33">
         <v>163</v>
       </c>
-      <c r="F52" s="33">
+      <c r="F52" s="20">
         <v>3</v>
       </c>
       <c r="G52" s="51">
-        <f>E52-F58</f>
-        <v>160</v>
+        <f>E52-SUM(F52:F58)</f>
+        <v>145</v>
       </c>
       <c r="H52" s="12"/>
     </row>
     <row r="53" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="44"/>
-      <c r="B53" s="34" t="s">
+      <c r="A53" s="25"/>
+      <c r="B53" s="21" t="s">
         <v>53</v>
       </c>
       <c r="C53" s="11">
         <v>41336</v>
       </c>
-      <c r="D53" s="32"/>
-      <c r="E53" s="49"/>
-      <c r="F53" s="33">
+      <c r="D53" s="19"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="20">
         <v>1</v>
       </c>
       <c r="G53" s="52"/>
       <c r="H53" s="12"/>
     </row>
     <row r="54" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="44"/>
-      <c r="B54" s="34" t="s">
+      <c r="A54" s="25"/>
+      <c r="B54" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C54" s="40" t="s">
+      <c r="C54" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D54" s="32"/>
-      <c r="E54" s="49"/>
-      <c r="F54" s="33">
+      <c r="D54" s="19"/>
+      <c r="E54" s="34"/>
+      <c r="F54" s="20">
         <v>2</v>
       </c>
       <c r="G54" s="52"/>
       <c r="H54" s="12"/>
     </row>
     <row r="55" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="44"/>
-      <c r="B55" s="34" t="s">
+      <c r="A55" s="25"/>
+      <c r="B55" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C55" s="11">
         <v>41336</v>
       </c>
-      <c r="D55" s="32"/>
-      <c r="E55" s="49"/>
-      <c r="F55" s="33">
+      <c r="D55" s="19"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="20">
         <v>3</v>
       </c>
       <c r="G55" s="52"/>
       <c r="H55" s="12"/>
     </row>
     <row r="56" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="44"/>
-      <c r="B56" s="34" t="s">
+      <c r="A56" s="25"/>
+      <c r="B56" s="21" t="s">
         <v>51</v>
       </c>
       <c r="C56" s="11">
         <v>41336</v>
       </c>
-      <c r="D56" s="32"/>
-      <c r="E56" s="49"/>
-      <c r="F56" s="33">
+      <c r="D56" s="19"/>
+      <c r="E56" s="34"/>
+      <c r="F56" s="20">
         <v>4</v>
       </c>
       <c r="G56" s="52"/>
       <c r="H56" s="12"/>
     </row>
     <row r="57" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="44"/>
-      <c r="B57" s="29" t="s">
+      <c r="A57" s="25"/>
+      <c r="B57" s="16" t="s">
         <v>47</v>
       </c>
       <c r="C57" s="13"/>
-      <c r="D57" s="32"/>
-      <c r="E57" s="49"/>
-      <c r="F57" s="33">
+      <c r="D57" s="19"/>
+      <c r="E57" s="34"/>
+      <c r="F57" s="20">
         <v>2</v>
       </c>
       <c r="G57" s="52"/>
       <c r="H57" s="12"/>
     </row>
     <row r="58" spans="1:8" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="39"/>
-      <c r="B58" s="29" t="s">
+      <c r="A58" s="26"/>
+      <c r="B58" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C58" s="30" t="s">
+      <c r="C58" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D58" s="31"/>
-      <c r="E58" s="50"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="35"/>
       <c r="F58" s="14">
         <v>3</v>
       </c>
@@ -2040,10 +2048,10 @@
       <c r="A59" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B59" s="16" t="s">
+      <c r="B59" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="C59" s="16"/>
+      <c r="C59" s="50"/>
       <c r="D59" s="7"/>
       <c r="E59" s="10">
         <f>SUM(E12:E28)</f>
@@ -2057,10 +2065,10 @@
       <c r="A60" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B60" s="16" t="s">
+      <c r="B60" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="C60" s="16"/>
+      <c r="C60" s="50"/>
       <c r="D60" s="7"/>
       <c r="E60" s="10">
         <f>SUM(E29:E45)</f>
@@ -2074,12 +2082,12 @@
       <c r="A61" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B61" s="16" t="s">
+      <c r="B61" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C61" s="16"/>
+      <c r="C61" s="50"/>
       <c r="D61" s="7"/>
-      <c r="E61" s="28">
+      <c r="E61" s="15">
         <f>SUM(E46:E57)</f>
         <v>319</v>
       </c>
@@ -2091,11 +2099,12 @@
       <c r="A62" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B62" s="16"/>
-      <c r="C62" s="16"/>
+      <c r="B62" s="50"/>
+      <c r="C62" s="50"/>
       <c r="D62" s="7"/>
       <c r="E62" s="10">
-        <v>1440</v>
+        <f>SUM(E59:E61)</f>
+        <v>1298</v>
       </c>
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
@@ -2112,71 +2121,71 @@
       <c r="H63" s="12"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="17" t="s">
+      <c r="A64" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="B64" s="17"/>
-      <c r="C64" s="17"/>
-      <c r="D64" s="17"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="17"/>
-      <c r="G64" s="17"/>
+      <c r="B64" s="39"/>
+      <c r="C64" s="39"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="39"/>
+      <c r="F64" s="39"/>
+      <c r="G64" s="39"/>
       <c r="H64" s="4"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="18" t="s">
+      <c r="A65" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B65" s="18" t="s">
+      <c r="B65" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C65" s="18" t="s">
+      <c r="C65" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="D65" s="18"/>
-      <c r="E65" s="18"/>
-      <c r="F65" s="18"/>
-      <c r="G65" s="18"/>
+      <c r="D65" s="40"/>
+      <c r="E65" s="40"/>
+      <c r="F65" s="40"/>
+      <c r="G65" s="40"/>
       <c r="H65" s="12"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="18"/>
-      <c r="B66" s="18"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="18"/>
-      <c r="F66" s="18"/>
-      <c r="G66" s="18"/>
+      <c r="A66" s="40"/>
+      <c r="B66" s="40"/>
+      <c r="C66" s="40"/>
+      <c r="D66" s="40"/>
+      <c r="E66" s="40"/>
+      <c r="F66" s="40"/>
+      <c r="G66" s="40"/>
       <c r="H66" s="12"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" s="15"/>
+      <c r="A67" s="41"/>
       <c r="B67" s="7"/>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="15"/>
-      <c r="F67" s="15"/>
-      <c r="G67" s="15"/>
+      <c r="C67" s="41"/>
+      <c r="D67" s="41"/>
+      <c r="E67" s="41"/>
+      <c r="F67" s="41"/>
+      <c r="G67" s="41"/>
       <c r="H67" s="12"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="15"/>
+      <c r="A68" s="41"/>
       <c r="B68" s="7"/>
-      <c r="C68" s="15"/>
-      <c r="D68" s="15"/>
-      <c r="E68" s="15"/>
-      <c r="F68" s="15"/>
-      <c r="G68" s="15"/>
+      <c r="C68" s="41"/>
+      <c r="D68" s="41"/>
+      <c r="E68" s="41"/>
+      <c r="F68" s="41"/>
+      <c r="G68" s="41"/>
       <c r="H68" s="12"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
-      <c r="C69" s="15"/>
-      <c r="D69" s="15"/>
-      <c r="E69" s="15"/>
-      <c r="F69" s="15"/>
-      <c r="G69" s="15"/>
+      <c r="C69" s="41"/>
+      <c r="D69" s="41"/>
+      <c r="E69" s="41"/>
+      <c r="F69" s="41"/>
+      <c r="G69" s="41"/>
       <c r="H69" s="12"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
@@ -2191,46 +2200,6 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="G29:G33"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="E29:E33"/>
-    <mergeCell ref="A52:A58"/>
-    <mergeCell ref="A46:A51"/>
-    <mergeCell ref="E46:E51"/>
-    <mergeCell ref="E52:E58"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="E12:E17"/>
-    <mergeCell ref="G12:G17"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="E18:E23"/>
-    <mergeCell ref="G18:G23"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="E24:E28"/>
-    <mergeCell ref="G24:G28"/>
-    <mergeCell ref="A34:A38"/>
-    <mergeCell ref="E34:E38"/>
-    <mergeCell ref="G34:G38"/>
-    <mergeCell ref="A39:A45"/>
-    <mergeCell ref="E39:E45"/>
-    <mergeCell ref="G39:G45"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="G52:G58"/>
-    <mergeCell ref="G46:G51"/>
     <mergeCell ref="A67:A68"/>
     <mergeCell ref="C67:G67"/>
     <mergeCell ref="C68:G68"/>
@@ -2240,6 +2209,46 @@
     <mergeCell ref="A65:A66"/>
     <mergeCell ref="B65:B66"/>
     <mergeCell ref="C65:G66"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="G52:G58"/>
+    <mergeCell ref="G46:G51"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="E18:E23"/>
+    <mergeCell ref="G18:G23"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="G24:G28"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="E12:E17"/>
+    <mergeCell ref="G12:G17"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="G29:G33"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="E29:E33"/>
+    <mergeCell ref="A52:A58"/>
+    <mergeCell ref="A46:A51"/>
+    <mergeCell ref="E46:E51"/>
+    <mergeCell ref="E52:E58"/>
+    <mergeCell ref="A34:A38"/>
+    <mergeCell ref="E34:E38"/>
+    <mergeCell ref="G34:G38"/>
+    <mergeCell ref="A39:A45"/>
+    <mergeCell ref="E39:E45"/>
+    <mergeCell ref="G39:G45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>